<commit_message>
finishing template excel duk
</commit_message>
<xml_diff>
--- a/public/files/template/kepegawaian/duk.xlsx
+++ b/public/files/template/kepegawaian/duk.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16828"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projek\epuskesmasgarut\public\files\template\kepegawaian\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\public_html\infokes\mprogram_garut\public\files\template\kepegawaian\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -324,7 +324,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -364,6 +364,66 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -381,65 +441,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="justify" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -535,23 +550,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -587,23 +585,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -759,169 +740,173 @@
   <dimension ref="A1:T15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="19" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" style="37" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" style="37" customWidth="1"/>
-    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" customWidth="1"/>
-    <col min="14" max="14" width="16.28515625" customWidth="1"/>
-    <col min="19" max="19" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="31.5703125" style="19" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="19" customWidth="1"/>
+    <col min="9" max="10" width="6.5703125" customWidth="1"/>
+    <col min="11" max="11" width="22.7109375" style="19" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" customWidth="1"/>
+    <col min="14" max="14" width="28.42578125" style="19" customWidth="1"/>
+    <col min="15" max="15" width="7.7109375" customWidth="1"/>
+    <col min="16" max="16" width="8.5703125" customWidth="1"/>
+    <col min="17" max="18" width="7.5703125" customWidth="1"/>
+    <col min="19" max="19" width="16.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
-      <c r="B1" s="5"/>
+      <c r="B1" s="45"/>
       <c r="C1" s="5"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="34"/>
+      <c r="F1" s="16"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="34"/>
+      <c r="H1" s="16"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
-      <c r="K1" s="1"/>
+      <c r="K1" s="16"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
+      <c r="N1" s="16"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
     </row>
     <row r="2" spans="1:20" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="36"/>
     </row>
     <row r="3" spans="1:20" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
-      <c r="T3" s="16"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="36"/>
+      <c r="O3" s="36"/>
+      <c r="P3" s="36"/>
+      <c r="Q3" s="36"/>
+      <c r="R3" s="36"/>
+      <c r="S3" s="36"/>
+      <c r="T3" s="36"/>
     </row>
     <row r="4" spans="1:20" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16"/>
-      <c r="T4" s="16"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="36"/>
+      <c r="Q4" s="36"/>
+      <c r="R4" s="36"/>
+      <c r="S4" s="36"/>
+      <c r="T4" s="36"/>
     </row>
     <row r="5" spans="1:20" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="35"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="35"/>
+      <c r="H5" s="17"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
+      <c r="K5" s="17"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
+      <c r="N5" s="17"/>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="4"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="17"/>
     </row>
     <row r="6" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="12" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="35"/>
+      <c r="F6" s="17"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="35"/>
+      <c r="H6" s="17"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
+      <c r="K6" s="17"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
+      <c r="N6" s="17"/>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="17"/>
     </row>
     <row r="7" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="11" t="s">
         <v>4</v>
       </c>
@@ -929,25 +914,25 @@
         <v>45</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="F7" s="35"/>
+      <c r="F7" s="17"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="35"/>
+      <c r="H7" s="17"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
+      <c r="K7" s="17"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
+      <c r="N7" s="17"/>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="17"/>
     </row>
     <row r="8" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="11" t="s">
         <v>2</v>
       </c>
@@ -955,25 +940,25 @@
         <v>44</v>
       </c>
       <c r="E8" s="13"/>
-      <c r="F8" s="35"/>
+      <c r="F8" s="17"/>
       <c r="G8" s="13"/>
-      <c r="H8" s="35"/>
+      <c r="H8" s="17"/>
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
+      <c r="K8" s="17"/>
       <c r="L8" s="13"/>
       <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
+      <c r="N8" s="17"/>
       <c r="O8" s="13"/>
       <c r="P8" s="13"/>
       <c r="Q8" s="13"/>
       <c r="R8" s="13"/>
-      <c r="S8" s="13"/>
-      <c r="T8" s="13"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="17"/>
     </row>
     <row r="9" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
+      <c r="B9" s="45"/>
       <c r="C9" s="11" t="s">
         <v>5</v>
       </c>
@@ -981,73 +966,73 @@
         <v>46</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="34"/>
+      <c r="F9" s="16"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="34"/>
+      <c r="H9" s="16"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="1"/>
+      <c r="K9" s="16"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
+      <c r="N9" s="16"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
     </row>
     <row r="10" spans="1:20" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
+      <c r="B10" s="45"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="34"/>
+      <c r="F10" s="16"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="34"/>
+      <c r="H10" s="16"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="1"/>
+      <c r="K10" s="16"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
+      <c r="N10" s="16"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
     </row>
     <row r="11" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="32" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="31" t="s">
+      <c r="E11" s="37"/>
+      <c r="F11" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="32"/>
-      <c r="H11" s="33"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="29"/>
       <c r="I11" s="6" t="s">
         <v>8</v>
       </c>
       <c r="J11" s="6"/>
-      <c r="K11" s="18" t="s">
+      <c r="K11" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="7" t="s">
+      <c r="L11" s="38"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="43" t="s">
         <v>10</v>
       </c>
       <c r="O11" s="7"/>
@@ -1056,54 +1041,54 @@
         <v>11</v>
       </c>
       <c r="R11" s="8"/>
-      <c r="S11" s="24" t="s">
+      <c r="S11" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="T11" s="24" t="s">
+      <c r="T11" s="32" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="29" t="s">
+      <c r="A12" s="40"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="30" t="s">
         <v>15</v>
       </c>
       <c r="E12" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="32" t="s">
         <v>13</v>
       </c>
       <c r="G12" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="22" t="s">
+      <c r="H12" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="I12" s="26" t="s">
+      <c r="I12" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="J12" s="26" t="s">
+      <c r="J12" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="K12" s="24" t="s">
+      <c r="K12" s="32" t="s">
         <v>13</v>
       </c>
       <c r="L12" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="M12" s="22" t="s">
+      <c r="M12" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="N12" s="24" t="s">
+      <c r="N12" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="O12" s="22" t="s">
+      <c r="O12" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="P12" s="22" t="s">
+      <c r="P12" s="32" t="s">
         <v>20</v>
       </c>
       <c r="Q12" s="24" t="s">
@@ -1112,36 +1097,36 @@
       <c r="R12" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="S12" s="28"/>
-      <c r="T12" s="28"/>
+      <c r="S12" s="44"/>
+      <c r="T12" s="44"/>
     </row>
     <row r="13" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="25"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="25"/>
-      <c r="R13" s="25"/>
-      <c r="S13" s="25"/>
-      <c r="T13" s="25"/>
+      <c r="A13" s="41"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="33"/>
+      <c r="O13" s="33"/>
+      <c r="P13" s="33"/>
+      <c r="Q13" s="26"/>
+      <c r="R13" s="26"/>
+      <c r="S13" s="33"/>
+      <c r="T13" s="33"/>
     </row>
     <row r="14" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>1</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="46">
         <v>2</v>
       </c>
       <c r="C14" s="9"/>
@@ -1151,13 +1136,13 @@
       <c r="E14" s="3">
         <v>5</v>
       </c>
-      <c r="F14" s="36">
+      <c r="F14" s="18">
         <v>6</v>
       </c>
       <c r="G14" s="3">
         <v>7</v>
       </c>
-      <c r="H14" s="36">
+      <c r="H14" s="18">
         <v>8</v>
       </c>
       <c r="I14" s="3">
@@ -1166,7 +1151,7 @@
       <c r="J14" s="3">
         <v>10</v>
       </c>
-      <c r="K14" s="3">
+      <c r="K14" s="18">
         <v>11</v>
       </c>
       <c r="L14" s="3">
@@ -1175,7 +1160,7 @@
       <c r="M14" s="3">
         <v>13</v>
       </c>
-      <c r="N14" s="3">
+      <c r="N14" s="18">
         <v>14</v>
       </c>
       <c r="O14" s="3">
@@ -1190,87 +1175,77 @@
       <c r="R14" s="3">
         <v>18</v>
       </c>
-      <c r="S14" s="3">
+      <c r="S14" s="18">
         <v>19</v>
       </c>
-      <c r="T14" s="3">
+      <c r="T14" s="18">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:20" s="40" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
+    <row r="15" spans="1:20" s="22" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="38" t="s">
+      <c r="C15" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="38" t="s">
+      <c r="D15" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="38" t="s">
+      <c r="E15" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="F15" s="39" t="s">
+      <c r="F15" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="38" t="s">
+      <c r="G15" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="41" t="s">
+      <c r="H15" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="I15" s="38" t="s">
+      <c r="I15" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="J15" s="38" t="s">
+      <c r="J15" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="K15" s="38" t="s">
+      <c r="K15" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="L15" s="38" t="s">
+      <c r="L15" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="M15" s="38" t="s">
+      <c r="M15" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="N15" s="38" t="s">
+      <c r="N15" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="O15" s="38" t="s">
+      <c r="O15" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="P15" s="38" t="s">
+      <c r="P15" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="Q15" s="38" t="s">
+      <c r="Q15" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="R15" s="38" t="s">
+      <c r="R15" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="S15" s="38" t="s">
+      <c r="S15" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="T15" s="38" t="s">
+      <c r="T15" s="21" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="S11:S13"/>
-    <mergeCell ref="T11:T13"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="Q12:Q13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:I13"/>
     <mergeCell ref="A2:T2"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="K11:M11"/>
@@ -1287,6 +1262,16 @@
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="R12:R13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="S11:S13"/>
+    <mergeCell ref="T11:T13"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="Q12:Q13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>